<commit_message>
[taekwon] spell_combine 버그 수정
ID 오류
</commit_message>
<xml_diff>
--- a/GameData/Excel/spell_combine.xlsx
+++ b/GameData/Excel/spell_combine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\문서\GitHub\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06D134F-1071-4A11-BD21-3464297F37AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ABF56E-DC4D-4ED3-A34A-09DE2500E52B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="345" windowWidth="46290" windowHeight="25680" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
@@ -625,8 +625,8 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -703,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="1">
-        <v>20201</v>
+        <v>20101</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="1">
-        <v>20202</v>
+        <v>20102</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
@@ -743,7 +743,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="1">
-        <v>20203</v>
+        <v>20103</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>17</v>
@@ -763,7 +763,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="1">
-        <v>20204</v>
+        <v>20104</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>18</v>
@@ -783,7 +783,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="1">
-        <v>20205</v>
+        <v>20105</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>19</v>
@@ -803,7 +803,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="1">
-        <v>20206</v>
+        <v>20106</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>20</v>
@@ -823,7 +823,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="1">
-        <v>20207</v>
+        <v>20107</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>21</v>
@@ -843,7 +843,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="1">
-        <v>20208</v>
+        <v>20108</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>22</v>
@@ -863,7 +863,7 @@
         <v>14</v>
       </c>
       <c r="E12" s="1">
-        <v>20209</v>
+        <v>20109</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>23</v>
@@ -883,7 +883,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="1">
-        <v>20210</v>
+        <v>20110</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>24</v>
@@ -1212,5 +1212,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>